<commit_message>
Table updates and SEM
</commit_message>
<xml_diff>
--- a/R1/Tables_R1.xlsx
+++ b/R1/Tables_R1.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hhan19/Documents/GitHub/COVIDiSTRESS2_Stress/R1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1EA789-9529-D242-B50B-521CFCDDD230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB269DA-5705-EC4C-8072-41741623B4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="980" windowWidth="29920" windowHeight="17220" activeTab="6" xr2:uid="{45521D96-D60F-B240-A4F7-C3951CE80050}"/>
+    <workbookView xWindow="7120" yWindow="680" windowWidth="29920" windowHeight="17220" activeTab="6" xr2:uid="{45521D96-D60F-B240-A4F7-C3951CE80050}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model BFs" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="1" r:id="rId1"/>
     <sheet name="Hypotheses" sheetId="2" r:id="rId2"/>
-    <sheet name="Mediation" sheetId="4" r:id="rId3"/>
-    <sheet name="Supp Model BFs" sheetId="5" r:id="rId4"/>
-    <sheet name="Supp Hypothesis" sheetId="6" r:id="rId5"/>
-    <sheet name="Supp Mediation" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="3" sheetId="10" r:id="rId3"/>
+    <sheet name="4" sheetId="11" r:id="rId4"/>
+    <sheet name="5" sheetId="12" r:id="rId5"/>
+    <sheet name="6" sheetId="13" r:id="rId6"/>
+    <sheet name="Mediation" sheetId="4" r:id="rId7"/>
+    <sheet name="Supp Model BFs" sheetId="5" r:id="rId8"/>
+    <sheet name="Supp Hypothesis" sheetId="6" r:id="rId9"/>
+    <sheet name="Supp Mediation" sheetId="7" r:id="rId10"/>
+    <sheet name="Correlation" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="78">
   <si>
     <t>log Model BF</t>
   </si>
@@ -72,18 +76,6 @@
   </si>
   <si>
     <t>Infinite</t>
-  </si>
-  <si>
-    <t>Best model without 
-random effects vs. M0</t>
-  </si>
-  <si>
-    <t>Best model without 
-random effects vs. M1</t>
-  </si>
-  <si>
-    <t>Best model without 
-random effects vs. M2</t>
   </si>
   <si>
     <t>M2</t>
@@ -272,6 +264,44 @@
   </si>
   <si>
     <t>6. Resilience</t>
+  </si>
+  <si>
+    <t>Best model</t>
+  </si>
+  <si>
+    <t>Best model adjusted ICC</t>
+  </si>
+  <si>
+    <t>Best model conditional ICC</t>
+  </si>
+  <si>
+    <t>M1 vs. M0 (logBF)</t>
+  </si>
+  <si>
+    <t>M2 vs. M0 (logBF)</t>
+  </si>
+  <si>
+    <t>M2 vs. M1 (logBF)</t>
+  </si>
+  <si>
+    <t>Best model without 
+random effects vs. M0 (logBF)</t>
+  </si>
+  <si>
+    <t>Best model without 
+random effects vs. M1 (logBF)</t>
+  </si>
+  <si>
+    <t>Best model without 
+random effects vs. M2 (logBF)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>(H.groupid.mediation)
+Group identity
+→ Social support</t>
   </si>
 </sst>
 </file>
@@ -353,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,6 +454,11 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,8 +489,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,15 +806,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DAB844-0DA0-BF4B-B45A-D2ECE4C93F12}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -786,24 +822,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -825,7 +859,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -848,7 +882,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -871,7 +905,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3">
         <v>11.35</v>
@@ -893,94 +927,140 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B7" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="8">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3">
         <v>638.30085999999994</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" s="3">
         <v>378.82987000000003</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D9" s="3">
         <v>1959.6749</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E9" s="3">
         <v>1382.4873399999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F9" s="3">
         <v>14883.203799999999</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G9" s="3">
         <v>12668.13651</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
+    <row r="10" spans="1:7" ht="43" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="3">
         <v>-262.76</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="3">
         <v>-224.09746999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D10" s="3">
         <v>-199.23953</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
         <v>-167.22297</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F10" s="3">
         <v>-659.92764999999997</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G10" s="3">
         <v>-243.92885999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8">
+    <row r="11" spans="1:7" ht="43" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="8">
         <v>-274.14999999999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C11" s="8">
         <v>-224.58096</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D11" s="8">
         <v>-217.40655000000001</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E11" s="8">
         <v>-164.46897999999999</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F11" s="8">
         <v>-651.17623000000003</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G11" s="8">
         <v>-241.68190000000001</v>
       </c>
     </row>
@@ -995,12 +1075,514 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B481113D-739D-1848-9BAB-0E88AE6AA43C}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="12">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="C5" s="12">
+        <v>-0.23400000000000001</v>
+      </c>
+      <c r="D5" s="12">
+        <v>-0.157</v>
+      </c>
+      <c r="E5" s="12">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="F5" s="12">
+        <v>-0.113</v>
+      </c>
+      <c r="G5" s="12">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="12">
+        <v>-4.7E-2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="D6" s="12">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="E6" s="12">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="F6" s="12">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="G6" s="12">
+        <v>-5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.374</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="12">
+        <v>-0.24299999999999999</v>
+      </c>
+      <c r="C8" s="12">
+        <v>-0.28399999999999997</v>
+      </c>
+      <c r="D8" s="12">
+        <v>-0.20200000000000001</v>
+      </c>
+      <c r="E8" s="12">
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="F8" s="12">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="G8" s="12">
+        <v>-0.151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="23">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.25430000000000003</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.37940000000000002</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.34229999999999999</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.41649999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.248</v>
+      </c>
+      <c r="E13" s="12">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="F13" s="12">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E14" s="12">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F14" s="12">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="G14" s="12">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-0.22600000000000001</v>
+      </c>
+      <c r="C15" s="12">
+        <v>-0.249</v>
+      </c>
+      <c r="D15" s="12">
+        <v>-0.20200000000000001</v>
+      </c>
+      <c r="E15" s="12">
+        <v>-0.22600000000000001</v>
+      </c>
+      <c r="F15" s="12">
+        <v>-0.249</v>
+      </c>
+      <c r="G15" s="12">
+        <v>-0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.122</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="23">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="C17" s="23">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="D17" s="23">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.23980000000000001</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0.32569999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC303FD-217B-1142-97A9-B4D62A6E86D4}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="3.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="30"/>
+      <c r="B1" s="25">
+        <v>2</v>
+      </c>
+      <c r="C1" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1" s="25">
+        <v>4</v>
+      </c>
+      <c r="E1" s="25">
+        <v>5</v>
+      </c>
+      <c r="F1" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="21">
+        <v>0.38</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="21">
+        <v>-0.21</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C5" s="21">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.43</v>
+      </c>
+      <c r="D6" s="21">
+        <v>-0.22</v>
+      </c>
+      <c r="E6" s="21">
+        <v>-0.05</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="31">
+        <v>-0.13</v>
+      </c>
+      <c r="C7" s="31">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.33</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.23</v>
+      </c>
+      <c r="F7" s="31">
+        <v>-0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6339DF3E-3BEB-0348-98F8-9885E1CA7512}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,66 +1600,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30"/>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="31"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3">
         <v>0.23</v>
@@ -1101,29 +1683,29 @@
         <v>35.270000000000003</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="A5" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>-0.15</v>
@@ -1147,29 +1729,29 @@
         <v>30.45</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3">
         <v>-0.28999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="A7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0.36</v>
@@ -1193,29 +1775,29 @@
         <v>38.74</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J8" s="3">
         <v>0.76</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="A9" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>-0.19</v>
@@ -1239,7 +1821,7 @@
         <v>8153</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J10" s="3">
         <v>-0.2</v>
@@ -1247,7 +1829,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3">
         <v>-0.1</v>
@@ -1271,29 +1853,29 @@
         <v>8179</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J11" s="3">
         <v>-0.37</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="A12" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="12">
         <v>0.31</v>
@@ -1317,7 +1899,7 @@
         <v>38.5</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J13" s="12">
         <v>0.76</v>
@@ -1325,7 +1907,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="12">
         <v>-0.08</v>
@@ -1349,7 +1931,7 @@
         <v>18.899999999999999</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J14" s="12">
         <v>-0.13</v>
@@ -1357,7 +1939,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="12">
         <v>0.01</v>
@@ -1388,22 +1970,22 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="A16" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3">
         <v>-0.22</v>
@@ -1427,29 +2009,29 @@
         <v>6924</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J17" s="3">
         <v>-0.43</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="A18" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3">
         <v>0.19</v>
@@ -1473,7 +2055,7 @@
         <v>6993</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J19" s="3">
         <v>0.19</v>
@@ -1481,7 +2063,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3">
         <v>0.09</v>
@@ -1505,29 +2087,29 @@
         <v>7010</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J20" s="3">
         <v>0.31</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="A21" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="12">
         <v>-0.18</v>
@@ -1551,7 +2133,7 @@
         <v>6826</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J22" s="12">
         <v>-0.42</v>
@@ -1559,7 +2141,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23" s="12">
         <v>0.14000000000000001</v>
@@ -1583,7 +2165,7 @@
         <v>6831</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J23" s="12">
         <v>0.23</v>
@@ -1591,7 +2173,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B24" s="12">
         <v>-0.01</v>
@@ -1622,22 +2204,22 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
+      <c r="A25" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" s="12">
         <v>-0.31</v>
@@ -1661,7 +2243,7 @@
         <v>22.26</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J26" s="12">
         <v>-0.64</v>
@@ -1669,7 +2251,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B27" s="12">
         <v>-0.05</v>
@@ -1693,7 +2275,7 @@
         <v>36.630000000000003</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J27" s="12">
         <v>-0.05</v>
@@ -1701,7 +2283,7 @@
     </row>
     <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28" s="12">
         <v>0.2</v>
@@ -1725,29 +2307,29 @@
         <v>18.64</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J28" s="12">
         <v>0.401881818</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
+      <c r="A29" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" s="12">
         <v>0.1</v>
@@ -1771,7 +2353,7 @@
         <v>35.68</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J30" s="12">
         <v>0.15791464290000001</v>
@@ -1779,7 +2361,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" s="16">
         <v>0.25</v>
@@ -1803,7 +2385,7 @@
         <v>27.04</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J31" s="16">
         <v>0.49852551699999997</v>
@@ -1811,7 +2393,7 @@
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B32" s="13">
         <v>0.2</v>
@@ -1835,7 +2417,7 @@
         <v>18.64</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J32" s="13">
         <v>0.401881818</v>
@@ -1868,11 +2450,1133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0D3F95-569B-A445-9E8D-20E2E749CCA9}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="A1:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G4" s="3">
+        <v>13.69</v>
+      </c>
+      <c r="H4" s="3">
+        <v>35.270000000000003</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8">
+        <v>-0.15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8">
+        <v>-0.17</v>
+      </c>
+      <c r="F6" s="8">
+        <v>-0.12</v>
+      </c>
+      <c r="G6" s="8">
+        <v>-8.93</v>
+      </c>
+      <c r="H6" s="8">
+        <v>30.45</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="8">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481AB138-C25F-C84E-B3D5-D84FF4AC9AD3}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>18.88</v>
+      </c>
+      <c r="H4" s="3">
+        <v>38.74</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-9.3800000000000008</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8153</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-0.11</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-16.09</v>
+      </c>
+      <c r="H7" s="3">
+        <v>8179</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="3">
+        <v>-0.37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.31</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.34</v>
+      </c>
+      <c r="G9" s="12">
+        <v>19.11</v>
+      </c>
+      <c r="H9" s="12">
+        <v>38.5</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="12">
+        <v>-0.08</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12">
+        <v>-0.11</v>
+      </c>
+      <c r="F10" s="12">
+        <v>-0.06</v>
+      </c>
+      <c r="G10" s="12">
+        <v>-5.95</v>
+      </c>
+      <c r="H10" s="12">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="12">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.23</v>
+      </c>
+      <c r="E11" s="13">
+        <v>-0.01</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1661</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0.44</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD96AF76-A5D7-234D-8386-839484BEE72B}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J11" sqref="A1:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-0.24</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="G4" s="3">
+        <v>-17.98</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6924</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7.86</v>
+      </c>
+      <c r="H6" s="3">
+        <v>6993</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G7" s="3">
+        <v>12.95</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7010</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="12">
+        <v>-0.18</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-0.2</v>
+      </c>
+      <c r="F9" s="12">
+        <v>-0.17</v>
+      </c>
+      <c r="G9" s="12">
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="H9" s="12">
+        <v>6826</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="12">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="G10" s="12">
+        <v>9.6</v>
+      </c>
+      <c r="H10" s="12">
+        <v>6831</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="13">
+        <v>-0.01</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="E11" s="13">
+        <v>-0.02</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="13">
+        <v>-0.71</v>
+      </c>
+      <c r="H11" s="13">
+        <v>6959</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0.48</v>
+      </c>
+      <c r="J11" s="13">
+        <v>-0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1AA7C-3E1B-5744-A052-6422E49AF1C8}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12">
+        <v>-0.31</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12">
+        <v>-0.34</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="G4" s="3">
+        <v>-17.991</v>
+      </c>
+      <c r="H4" s="12">
+        <v>22.26</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12">
+        <v>-0.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12">
+        <v>-0.05</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12">
+        <v>-0.08</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-3.7360000000000002</v>
+      </c>
+      <c r="H5" s="12">
+        <v>36.630000000000003</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="12">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.22</v>
+      </c>
+      <c r="G6" s="12">
+        <v>15.042999999999999</v>
+      </c>
+      <c r="H6" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0.401881818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="G8" s="12">
+        <v>7.4290000000000003</v>
+      </c>
+      <c r="H8" s="12">
+        <v>35.68</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.15791464290000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.22</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G9" s="16">
+        <v>12.723000000000001</v>
+      </c>
+      <c r="H9" s="16">
+        <v>27.04</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.49852551699999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.22</v>
+      </c>
+      <c r="G10" s="13">
+        <v>15.042999999999999</v>
+      </c>
+      <c r="H10" s="13">
+        <v>18.64</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0.401881818</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AFA510-D444-C649-8FCA-4E92763698E4}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1886,54 +3590,54 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
-      <c r="B1" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="36"/>
+      <c r="B2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="31"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="31"/>
+        <v>16</v>
+      </c>
+      <c r="E3" s="34"/>
       <c r="F3" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="21">
         <v>-0.05</v>
@@ -1956,7 +3660,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="21">
         <v>-6.0999999999999999E-2</v>
@@ -1979,7 +3683,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" s="21">
         <v>-0.311</v>
@@ -2002,7 +3706,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7" s="21">
         <v>-0.111</v>
@@ -2025,7 +3729,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8" s="23">
         <v>0.54879999999999995</v>
@@ -2056,10 +3760,11 @@
     <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC05D6C-FF2F-494A-BA73-11AD9F101604}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2079,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>5</v>
@@ -2120,13 +3825,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2134,7 +3839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EF42F5-2418-3D42-8752-AE10A8546C3D}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -2153,45 +3858,45 @@
   <sheetData>
     <row r="1" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
-      <c r="B1" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="30"/>
+      <c r="B1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="A3" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="12">
         <v>-0.2</v>
@@ -2211,7 +3916,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="12">
         <v>-0.1</v>
@@ -2231,7 +3936,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="12">
         <v>0.35</v>
@@ -2251,7 +3956,7 @@
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B7" s="12">
         <v>-0.13</v>
@@ -2271,7 +3976,7 @@
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" s="12">
         <v>-0.17</v>
@@ -2290,18 +3995,18 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="A9" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="12">
         <v>0.2</v>
@@ -2321,7 +4026,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="12">
         <v>0.1</v>
@@ -2341,7 +4046,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" s="12">
         <v>-0.23</v>
@@ -2361,7 +4066,7 @@
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="12">
         <v>-0.14000000000000001</v>
@@ -2381,7 +4086,7 @@
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="13">
         <v>-0.17</v>
@@ -2410,506 +4115,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B481113D-739D-1848-9BAB-0E88AE6AA43C}">
-  <dimension ref="A1:G17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="36"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="12">
-        <v>-0.19600000000000001</v>
-      </c>
-      <c r="C5" s="12">
-        <v>-0.23400000000000001</v>
-      </c>
-      <c r="D5" s="12">
-        <v>-0.157</v>
-      </c>
-      <c r="E5" s="12">
-        <v>-0.10100000000000001</v>
-      </c>
-      <c r="F5" s="12">
-        <v>-0.113</v>
-      </c>
-      <c r="G5" s="12">
-        <v>-8.8999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="12">
-        <v>-4.7E-2</v>
-      </c>
-      <c r="C6" s="12">
-        <v>-6.3E-2</v>
-      </c>
-      <c r="D6" s="12">
-        <v>-3.2000000000000001E-2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>-6.2E-2</v>
-      </c>
-      <c r="F6" s="12">
-        <v>-6.7000000000000004E-2</v>
-      </c>
-      <c r="G6" s="12">
-        <v>-5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.374</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0.374</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="12">
-        <v>-0.24299999999999999</v>
-      </c>
-      <c r="C8" s="12">
-        <v>-0.28399999999999997</v>
-      </c>
-      <c r="D8" s="12">
-        <v>-0.20200000000000001</v>
-      </c>
-      <c r="E8" s="12">
-        <v>-0.16300000000000001</v>
-      </c>
-      <c r="F8" s="12">
-        <v>-0.17499999999999999</v>
-      </c>
-      <c r="G8" s="12">
-        <v>-0.151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="23">
-        <v>0.19339999999999999</v>
-      </c>
-      <c r="C9" s="23">
-        <v>0.13250000000000001</v>
-      </c>
-      <c r="D9" s="23">
-        <v>0.25430000000000003</v>
-      </c>
-      <c r="E9" s="23">
-        <v>0.37940000000000002</v>
-      </c>
-      <c r="F9" s="23">
-        <v>0.34229999999999999</v>
-      </c>
-      <c r="G9" s="23">
-        <v>0.41649999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.248</v>
-      </c>
-      <c r="E13" s="12">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="F13" s="12">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0.111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="D14" s="12">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E14" s="12">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="F14" s="12">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G14" s="12">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="12">
-        <v>-0.22600000000000001</v>
-      </c>
-      <c r="C15" s="12">
-        <v>-0.249</v>
-      </c>
-      <c r="D15" s="12">
-        <v>-0.20200000000000001</v>
-      </c>
-      <c r="E15" s="12">
-        <v>-0.22600000000000001</v>
-      </c>
-      <c r="F15" s="12">
-        <v>-0.249</v>
-      </c>
-      <c r="G15" s="12">
-        <v>-0.20200000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="12">
-        <v>0.23</v>
-      </c>
-      <c r="C16" s="12">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0.122</v>
-      </c>
-      <c r="G16" s="12">
-        <v>0.14899999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="23">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="C17" s="23">
-        <v>8.0399999999999999E-2</v>
-      </c>
-      <c r="D17" s="23">
-        <v>0.18360000000000001</v>
-      </c>
-      <c r="E17" s="23">
-        <v>0.28270000000000001</v>
-      </c>
-      <c r="F17" s="23">
-        <v>0.23980000000000001</v>
-      </c>
-      <c r="G17" s="23">
-        <v>0.32569999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:G11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC303FD-217B-1142-97A9-B4D62A6E86D4}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="3.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="B1" s="25">
-        <v>2</v>
-      </c>
-      <c r="C1" s="25">
-        <v>3</v>
-      </c>
-      <c r="D1" s="25">
-        <v>4</v>
-      </c>
-      <c r="E1" s="25">
-        <v>5</v>
-      </c>
-      <c r="F1" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="21">
-        <v>0.38</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="C4" s="21">
-        <v>-0.21</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="21">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C5" s="21">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="D5" s="21">
-        <v>0.35</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="21">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C6" s="21">
-        <v>0.43</v>
-      </c>
-      <c r="D6" s="21">
-        <v>-0.22</v>
-      </c>
-      <c r="E6" s="21">
-        <v>-0.05</v>
-      </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="41">
-        <v>-0.13</v>
-      </c>
-      <c r="C7" s="41">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="D7" s="41">
-        <v>0.33</v>
-      </c>
-      <c r="E7" s="41">
-        <v>0.23</v>
-      </c>
-      <c r="F7" s="41">
-        <v>-0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>